<commit_message>
fix the csv not combining two task types
</commit_message>
<xml_diff>
--- a/high_confidence_for_annotation.xlsx
+++ b/high_confidence_for_annotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosydai/Desktop/Master_thesis/Frontend/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22675CB9-CD50-8441-8A10-86DD3F5B63E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B016491B-4D71-5744-A020-6E767432DB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17340" xr2:uid="{DC94E088-820A-3B47-AB40-7E8AE428A805}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Raziyeh_high_conf" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">toBeDone!$A$1:$K$451</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">toBeDone!$A$1:$K$450</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5101" uniqueCount="997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5076" uniqueCount="992">
   <si>
     <t>ID_int</t>
   </si>
@@ -3003,12 +3003,6 @@
     <t>IMPROVING_THE_PHASE_STABILITY_OF_THE.pdf</t>
   </si>
   <si>
-    <t>[6] J. W. Wang, "RF Properties of Periodic Accelerating Structures for Linear Colliders", SLAC-339, July 1989 [7] F.-J. Decker, D. Farkas, L. Rinolfi, J. Truher, "Reducing Energy Spread for Long Bunch Train at SLAC", SLAC-PUB-7214, June 1996.</t>
-  </si>
-  <si>
-    <t>STUDY_OF_A_BUNCH_TRAIN_TOTAL_ENERGY_SPREAD_IN_A_LINAC.pdf</t>
-  </si>
-  <si>
     <t>Three more accelerating structures were placed downstream of the first one with a distance between adjacent coupler centers of $0 . 3 5 \\mathrm { m }$ . The beam from the first structure at maximum brightness was used as input to that part of the linac but the reference particle was moved to the new bunch center. Phases of the three structures were set for maximum acceleration but with a phase offset of - $. 1 5 ^ { \\circ }$ to provide some additional longitudinal compression of the bunch. Figure 2 shows resulted longitudinal phase space cropped at the DR level. The accepted yield is $8 . 0 ~ \\mathrm { { n } _ { e + } / \\mathrm { { n } _ { e } - } }$ and the total yield is $8 . 6 ~ \\mathrm { { n } _ { e } + / \\mathrm { { n } _ { e } - } }$ . The root mean square (RMS) energy spread of accepted particles $\\Delta \\mathrm { W } / \\mathrm { W }$ is $1 . 1 \\%$ and RMS bunch length $\\Delta Z$ is $2 . 8 \\mathrm { m m }$ .</t>
   </si>
   <si>
@@ -3019,15 +3013,6 @@
   </si>
   <si>
     <t>ANALYTICAL_POTENTIAL_MODEL_FOR_THE_RADIO-FREQUENCY.pdf</t>
-  </si>
-  <si>
-    <t>[10] D. Breton, J. Malmii, WaveCatcher Family User‚Äôs Manual, 2017. [11] L. Burmistrov, D. Breton, V. Chaumat, S. Conforti Di Lorenzo, J. Jeglot, J. Maalmi, V. Puill, A. Stocchi, J. Vagnucci, G. Cavoto, M. Garattini, F. Iacoangeli, F.L.S. Montesano, W. Scandale, Cherenkov detector for proton flux measurement for ua9 project, in: 2013 IEEE Nuclear Science Symposium and Medical Imaging Conference (2013 NSS/MIC), 2013, pp. 1‚Äì4, http://dx.doi.org/10.1109/NSSMIC. 2013.6829430. [12] L. Burmistrov, D. Breton, G. Cavoto, V. Chaumat, J. Collin, S.C.D. Lorenzo, M. Garattini, F. Iacoangeli, J. Jeglot, J. Maalmi, S. Montesano, V. Puill, R. Rossi, W. Scandale, A. Stocchi, J.-F. Vagnucci, Test of full size cherenkov detector for proton flux measurements, Nucl. Instrum. Methods Phys. Res. A 787 (2015) 173‚Äì175, http://dx.doi.org/10.1016/j.nima.2014.11.089, new Developments in Photodetection NDIP14. URL http://www.sciencedirect.com/science/article/pii/ S016890021401403X. [13] F.M. Addesa, G. Cavoto, In-vacuum Cherenkov light detectors for crystal-assisted beam manipulations, presented 28 Sep 2018 (Jun 2018). URL https://cds.cern. ch/record/2661725. [14] S. Montesano, W. Scandale, Status and results of the UA9 crystal collimation experiment at the cern-sps, in: HB2012: Proceedings of the 52nd ICFA Advanced Beam Dynamics Workshop on High-Intensity and High-Brightness Hadron Beams, Beijing, China, Sept. 17-21, 2012, 2012, p. 245, URL https://accelconf.web.cern. ch/accelconf/HB2012/papers/tuo3a02.pdf. [15] A. Natochii, L. Burmistrov, F. Addesa, O. Bezshyyko, D. Breton, V. Chaumat, G. Cavoto, S. Dubos, Y. Gavrikov, F. Iacoangeli, J.M.D. Bello, S. Montesano, V. Puill, R. Rossi, W. Scandale, A. Stocchi, Characterisation of the fused silica surface quality with a $\\beta$ -source, Nucl. Instrum. Methods Phys. Res. A 910 (2018) 15‚Äì21, http://dx.doi.org/10.1016/j.nima.2018.08.119, URL http://www. sciencedirect.com/science/article/pii/S0168900218310775.</t>
-  </si>
-  <si>
-    <t>REFERENCES [1] L. Faillace et al., ‚ÄúStatus of compact inverse compton sources in Italy: BriXS and STAR,‚Äù in Advances in Laboratorybased X-Ray Sources, Optics, and Applications VII, International Society for Optics and Photonics, vol. 11110, 2019, p. 1 111 005. [2] V. Shiltsev and F. Zimmermann, ‚ÄúModern and future colliders,‚Äù Rev. Mod. Phys., vol. 93, p. 015 006, 2021. doi:10.1103/RevModPhys.93.015006 [3] L. Faillace et al., ‚ÄúPerspectives in linear accelerator for flash vhee: Study of a compact c-band system,‚Äù Physica Medica, vol. 104, pp. 149‚Äì159, 2022. doi:10.1016/j.ejmp.2022.10.018 [4] T. P. Wangler, RF Linear Accelerators. J. Wiley &amp; Sons, 2008. [5] A. D. Cahill, J. B. Rosenzweig, V. A. Dolgashev, Z. Li, S. G. Tantawi, and S. Weathersby, ‚ÄúRf losses in a high gradient cryogenic copper cavity,‚Äù Phys. Rev. Accel. Beams, vol. 21, p. 061 301, 6 2018. doi:10.1103/PhysRevAccelBeams.21.061301 [6] A. D. Cahill, J. B. Rosenzweig, V. A. Dolgashev, S. G. Tantawi, and S. Weathersby, ‚ÄúHigh gradient experiments with X-band cryogenic copper accelerating cavities,‚Äù Phys. Rev. Accel. Beams, vol. 21, p. 102 002, 10 2018. doi:10.1103/PhysRevAccelBeams.21.102002 [7] S. Tantawi, M. Nasr, Z. Li, C. Limborg, and P. Borchard, ‚ÄúDesign and demonstration of a distributed-coupling linear accelerator structure,‚Äù Phys. Rev. Accel. Beams, vol. 23, no. 9, p. 092 001, 2020.</t>
-  </si>
-  <si>
-    <t>PRELIMINARYTESTS_FORTHE_DIFFUSIONBONDINGOF.pdf</t>
   </si>
   <si>
     <t>Daisy</t>
@@ -3445,18 +3430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A85F72-B3EC-EB4D-A3E1-C70AFE08A3AE}">
-  <dimension ref="A1:J455"/>
+  <dimension ref="A1:J452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B436" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B435" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E463" sqref="E463"/>
+      <selection pane="bottomRight" activeCell="A451" sqref="A451:A452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -17576,31 +17562,31 @@
         <v>864</v>
       </c>
       <c r="B442" s="2">
-        <v>1323</v>
+        <v>1687</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D442" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E442" t="s">
         <v>306</v>
       </c>
       <c r="F442" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="G442" t="s">
         <v>160</v>
       </c>
       <c r="H442" t="s">
-        <v>987</v>
+        <v>692</v>
       </c>
       <c r="I442" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="J442" t="s">
-        <v>988</v>
+        <v>866</v>
       </c>
     </row>
     <row r="443" spans="1:10" x14ac:dyDescent="0.2">
@@ -17608,13 +17594,13 @@
         <v>864</v>
       </c>
       <c r="B443" s="2">
-        <v>1687</v>
+        <v>1737</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D443" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E443" t="s">
         <v>306</v>
@@ -17626,13 +17612,13 @@
         <v>160</v>
       </c>
       <c r="H443" t="s">
-        <v>692</v>
+        <v>987</v>
       </c>
       <c r="I443" t="s">
         <v>757</v>
       </c>
       <c r="J443" t="s">
-        <v>866</v>
+        <v>988</v>
       </c>
     </row>
     <row r="444" spans="1:10" x14ac:dyDescent="0.2">
@@ -17640,31 +17626,31 @@
         <v>864</v>
       </c>
       <c r="B444" s="2">
-        <v>1737</v>
+        <v>2457</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D444" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E444" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F444" t="s">
-        <v>417</v>
+        <v>536</v>
       </c>
       <c r="G444" t="s">
-        <v>160</v>
+        <v>563</v>
       </c>
       <c r="H444" t="s">
-        <v>989</v>
+        <v>894</v>
       </c>
       <c r="I444" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="J444" t="s">
-        <v>990</v>
+        <v>866</v>
       </c>
     </row>
     <row r="445" spans="1:10" x14ac:dyDescent="0.2">
@@ -17672,7 +17658,7 @@
         <v>864</v>
       </c>
       <c r="B445" s="2">
-        <v>2457</v>
+        <v>2490</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>866</v>
@@ -17690,7 +17676,7 @@
         <v>563</v>
       </c>
       <c r="H445" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="I445" t="s">
         <v>758</v>
@@ -17704,13 +17690,13 @@
         <v>864</v>
       </c>
       <c r="B446" s="2">
-        <v>2490</v>
+        <v>2501</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D446" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E446" t="s">
         <v>298</v>
@@ -17722,13 +17708,13 @@
         <v>563</v>
       </c>
       <c r="H446" t="s">
-        <v>896</v>
+        <v>989</v>
       </c>
       <c r="I446" t="s">
         <v>758</v>
       </c>
       <c r="J446" t="s">
-        <v>866</v>
+        <v>990</v>
       </c>
     </row>
     <row r="447" spans="1:10" x14ac:dyDescent="0.2">
@@ -17736,7 +17722,7 @@
         <v>864</v>
       </c>
       <c r="B447" s="2">
-        <v>2501</v>
+        <v>2599</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>866</v>
@@ -17748,19 +17734,19 @@
         <v>298</v>
       </c>
       <c r="F447" t="s">
-        <v>536</v>
+        <v>438</v>
       </c>
       <c r="G447" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="H447" t="s">
-        <v>991</v>
+        <v>610</v>
       </c>
       <c r="I447" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="J447" t="s">
-        <v>992</v>
+        <v>782</v>
       </c>
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.2">
@@ -17768,31 +17754,31 @@
         <v>864</v>
       </c>
       <c r="B448" s="2">
-        <v>2599</v>
+        <v>3949</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D448" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E448" t="s">
         <v>298</v>
       </c>
       <c r="F448" t="s">
-        <v>438</v>
+        <v>480</v>
       </c>
       <c r="G448" t="s">
         <v>565</v>
       </c>
       <c r="H448" t="s">
-        <v>610</v>
+        <v>912</v>
       </c>
       <c r="I448" t="s">
         <v>756</v>
       </c>
       <c r="J448" t="s">
-        <v>782</v>
+        <v>866</v>
       </c>
     </row>
     <row r="449" spans="1:10" x14ac:dyDescent="0.2">
@@ -17800,63 +17786,57 @@
         <v>864</v>
       </c>
       <c r="B449" s="2">
-        <v>3207</v>
+        <v>8888</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D449" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E449" t="s">
-        <v>340</v>
+        <v>991</v>
       </c>
       <c r="F449" t="s">
-        <v>550</v>
+        <v>438</v>
       </c>
       <c r="G449" t="s">
-        <v>157</v>
+        <v>565</v>
       </c>
       <c r="H449" t="s">
-        <v>993</v>
+        <v>610</v>
       </c>
       <c r="I449" t="s">
-        <v>761</v>
-      </c>
-      <c r="J449" t="s">
-        <v>866</v>
+        <v>756</v>
       </c>
     </row>
     <row r="450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>864</v>
+        <v>834</v>
       </c>
       <c r="B450" s="2">
-        <v>3305</v>
+        <v>8888</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D450" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E450" t="s">
-        <v>306</v>
+        <v>991</v>
       </c>
       <c r="F450" t="s">
-        <v>466</v>
+        <v>480</v>
       </c>
       <c r="G450" t="s">
-        <v>159</v>
+        <v>565</v>
       </c>
       <c r="H450" t="s">
-        <v>994</v>
+        <v>912</v>
       </c>
       <c r="I450" t="s">
-        <v>762</v>
-      </c>
-      <c r="J450" t="s">
-        <v>995</v>
+        <v>756</v>
       </c>
     </row>
     <row r="451" spans="1:10" x14ac:dyDescent="0.2">
@@ -17864,36 +17844,36 @@
         <v>864</v>
       </c>
       <c r="B451" s="2">
-        <v>3949</v>
+        <v>8888</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>866</v>
       </c>
       <c r="D451" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E451" t="s">
-        <v>298</v>
+        <v>991</v>
       </c>
       <c r="F451" t="s">
-        <v>480</v>
+        <v>417</v>
       </c>
       <c r="G451" t="s">
-        <v>565</v>
+        <v>160</v>
       </c>
       <c r="H451" t="s">
-        <v>912</v>
+        <v>987</v>
       </c>
       <c r="I451" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="J451" t="s">
-        <v>866</v>
+        <v>988</v>
       </c>
     </row>
     <row r="452" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>864</v>
+        <v>834</v>
       </c>
       <c r="B452" s="2">
         <v>8888</v>
@@ -17902,119 +17882,35 @@
         <v>866</v>
       </c>
       <c r="D452" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E452" t="s">
-        <v>996</v>
+        <v>991</v>
       </c>
       <c r="F452" t="s">
-        <v>438</v>
+        <v>536</v>
       </c>
       <c r="G452" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H452" t="s">
-        <v>610</v>
+        <v>894</v>
       </c>
       <c r="I452" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A453" t="s">
-        <v>864</v>
-      </c>
-      <c r="B453" s="2">
-        <v>8888</v>
-      </c>
-      <c r="C453" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="J452" t="s">
         <v>866</v>
       </c>
-      <c r="D453" t="s">
-        <v>10</v>
-      </c>
-      <c r="E453" t="s">
-        <v>996</v>
-      </c>
-      <c r="F453" t="s">
-        <v>550</v>
-      </c>
-      <c r="G453" t="s">
-        <v>157</v>
-      </c>
-      <c r="H453" t="s">
-        <v>993</v>
-      </c>
-      <c r="I453" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A454" t="s">
-        <v>834</v>
-      </c>
-      <c r="B454" s="2">
-        <v>8888</v>
-      </c>
-      <c r="C454" s="2" t="s">
-        <v>866</v>
-      </c>
-      <c r="D454" t="s">
-        <v>22</v>
-      </c>
-      <c r="E454" t="s">
-        <v>996</v>
-      </c>
-      <c r="F454" t="s">
-        <v>466</v>
-      </c>
-      <c r="G454" t="s">
-        <v>159</v>
-      </c>
-      <c r="H454" t="s">
-        <v>994</v>
-      </c>
-      <c r="I454" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A455" t="s">
-        <v>834</v>
-      </c>
-      <c r="B455" s="2">
-        <v>8888</v>
-      </c>
-      <c r="C455" s="2" t="s">
-        <v>866</v>
-      </c>
-      <c r="D455" t="s">
-        <v>10</v>
-      </c>
-      <c r="E455" t="s">
-        <v>996</v>
-      </c>
-      <c r="F455" t="s">
-        <v>480</v>
-      </c>
-      <c r="G455" t="s">
-        <v>565</v>
-      </c>
-      <c r="H455" t="s">
-        <v>912</v>
-      </c>
-      <c r="I455" t="s">
-        <v>756</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K451" xr:uid="{B7A85F72-B3EC-EB4D-A3E1-C70AFE08A3AE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J451">
-      <sortCondition ref="A1:A451"/>
+  <autoFilter ref="A1:K450" xr:uid="{B7A85F72-B3EC-EB4D-A3E1-C70AFE08A3AE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J448">
+      <sortCondition ref="A1:A448"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="B246:B455">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="B246:B452">
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>